<commit_message>
actualización de datos y tasa de mortalidad
</commit_message>
<xml_diff>
--- a/public/covid-19-bd.xlsx
+++ b/public/covid-19-bd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\monitorsonora\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C4CEEE-D364-4104-8417-D2913D6CEAE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402ADF88-6174-4FE6-8D61-6193F328FED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17640" yWindow="510" windowWidth="20730" windowHeight="11760" xr2:uid="{69C15E0C-935F-4AD5-BC61-9BB5DD357911}"/>
+    <workbookView xWindow="21330" yWindow="3900" windowWidth="14745" windowHeight="8370" activeTab="2" xr2:uid="{69C15E0C-935F-4AD5-BC61-9BB5DD357911}"/>
   </bookViews>
   <sheets>
     <sheet name="Proporción" sheetId="1" r:id="rId1"/>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19192E84-C698-4952-81E5-A03EABB50D01}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1025,61 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11" si="56">C11+D11+E11+F11+G11</f>
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>59</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="I11" s="1">
+        <v>43934</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11" si="57">B11</f>
+        <v>88</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" ref="K11" si="58">C11/$B11</f>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" ref="L11" si="59">D11/$B11</f>
+        <v>0.67045454545454541</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" ref="M11" si="60">E11/$B11</f>
+        <v>5.6818181818181816E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11" si="61">F11/$B11</f>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" ref="O11" si="62">G11/$B11</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" ref="P11" si="63">SUM(K11:O11)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1032,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B806B08-CF1D-4A1B-A4AE-551FE020B3F7}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,6 +1527,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B11">
+        <f>SUM(C11:M11)</f>
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1479,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5465B67A-AEDE-4A88-9916-DBBF79ED193A}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,6 +1946,18 @@
         <v>86</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31" si="5">C30+B31</f>
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>